<commit_message>
Add some changes and comments.
</commit_message>
<xml_diff>
--- a/nesting_conopophagidae.xlsx
+++ b/nesting_conopophagidae.xlsx
@@ -17,6 +17,123 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="F27">
+      <text>
+        <t xml:space="preserve">"height of 40.6 ± 16.1 cm (range = 15–75) above the ground (N = 22).
+	-Odilon Vieira
+----
+Pereira et al. (2022): "40,6 ± 16,1 cm (N = 21)".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D27">
+      <text>
+        <t xml:space="preserve">"external diameter of 79.1 ± 11.1 mm (N = 21)".
+	-Odilon Vieira
+----
+Pereira et al. (2022): "79.1 ± 11.1 mm (n = 21)".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B27">
+      <text>
+        <t xml:space="preserve">"internal diameter of 59.4 ± 7.2 mm (N = 21)".
+	-Odilon Vieira
+----
+Pereira et al. (2022): "59.4 ± 7.2 mm (n = 21)".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="C27">
+      <text>
+        <t xml:space="preserve">"depth of 40.6 ± 16.1 mm (N = 21)".
+	-Odilon Vieira
+----
+Pereira et al. (2022): "40.6 ± 16.1 mm (n = 21)".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="E13">
+      <text>
+        <t xml:space="preserve">"8.6 cm ± 0.35 SE for cup height (N = 58)".
+	-Odilon Vieira
+----
+Studer et al. (2019): "8.6 cm ± 0.35 SE n = 58".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="C13">
+      <text>
+        <t xml:space="preserve">"3.78 cm ± 0.25 SE for depth of nest cup (N = 58)".
+	-Odilon Vieira
+----
+Studer et al. (2019): "3.78 cm ± 0.25 SE n = 58".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B13">
+      <text>
+        <t xml:space="preserve">"6.11 cm ± 0.14 SE internal diameter (N = 58)".
+	-Odilon Vieira
+----
+Studer et al. (2019): "6.11 cm ± 0.14 SE n = 58".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D13">
+      <text>
+        <t xml:space="preserve">"13.6 cm ± 0.54 SE external diameter (N = 58)".
+	-Odilon Vieira
+----
+Studer et al. (2019): "13.6 cm ± 0.54 SE n = 58".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="F13">
+      <text>
+        <t xml:space="preserve">"Heights above ground ranged from 30 to 265 cm (x̅ = 69.4cm; ± 4.33 SE; N = 99)".
+	-Odilon Vieira
+----
+Studer et al. 2019: "Heights above ground ranged from 30 to 265 cm (x̅ = 69.4cm; ± 4.33 SE; N = 99)".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="F41">
+      <text>
+        <t xml:space="preserve">"entre 20 e 50 cm do solo (0,35 ± 0,11 cm, n = 7)".
+	-Odilon Vieira
+----
+Marini et al. (2007): "0,35 ± 0,11 cm, (n = 7), 20-50".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="C41">
+      <text>
+        <t xml:space="preserve">"5,1 ± 0,3 cm de profundidade (n = 3)".
+	-Odilon Vieira
+----
+Marini et al. (2007): "5,1 ± 0,3 cm (n = 3)".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B41">
+      <text>
+        <t xml:space="preserve">"7,4 ± 0,4 cm de diâmetro interno (n = 4)"
+	-Odilon Vieira
+----
+Marini et al. (2007): "7,4 ± 0,4 cm (n = 4)".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D41">
+      <text>
+        <t xml:space="preserve">"12 ± 1,1 cm de diâmetro externo (n = 4)"
+	-Odilon Vieira
+----
+Marini et al. (2007): "12 ± 1,1 cm (n = 4)"
+	-Odilon Vieira</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="F40">
       <text>
         <t xml:space="preserve">Whitney (2003): "nearly 2 m".
@@ -63,6 +180,93 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="C83">
+      <text>
+        <t xml:space="preserve">" 17.9 ± 0.9 mm (N = 3)".
+	-Odilon Vieira
+----
+Lizarazo &amp; Londoño (2022): " 17.9 ± 0.9 mm (n = 3)".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B83">
+      <text>
+        <t xml:space="preserve">"22.5 ± 1.1 mm (N = 3)".
+	-Odilon Vieira
+----
+Lizarazo &amp; Londoño (2022): " 22.5 ± 1.1 mm (n = 3)".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="C39">
+      <text>
+        <t xml:space="preserve">"17.2 ± 0.8 mm (N = 23)".
+	-Odilon Vieira
+----
+Pereira et al. (2022): "17,2 ± 0,8 mm (n = 23)".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B39">
+      <text>
+        <t xml:space="preserve">"21.3 ± 0.8 mm (N = 23)".
+	-Odilon Vieira
+----
+Pereira et al. (2022): "21,3 ± 0,8 mm (n = 23)".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D14">
+      <text>
+        <t xml:space="preserve">"3.21g ± 0.1 SE (N = 40)".
+	-Odilon Vieira
+----
+Studer et al. (2019): "3.21g ± 0.1 SE (n = 40)".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B14">
+      <text>
+        <t xml:space="preserve">"22.41 mm ± 0.07 SE long (N = 41)".
+	-Odilon Vieira
+----
+Studer et al. (2019): "22.41 mm ± 0.07 SE (n = 41)".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="C14">
+      <text>
+        <t xml:space="preserve">"17.03 mm ± 0.08 SE wide (N = 41)".
+	-Odilon Vieira
+----
+Studer et al. (2019): "17.03 mm ± 0.08 SE (n = 41)".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="F66">
+      <text>
+        <t xml:space="preserve">"Three nests containing one, two and two eggs were found, [...]. A nest with four nestlings attended by at least one adult was found, ...".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="F63">
+      <text>
+        <t xml:space="preserve">"Doze ninhos foram encontrados, a maioria com dois ovos (n = 10), mas também registramos uma ninhada de um ovo e uma de três ovos".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D83">
+      <text>
+        <t xml:space="preserve">"3.9 ± 1.5 g (N = 3)"
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D39">
+      <text>
+        <t xml:space="preserve">"3.1 ± 0.1 g (N = 23)".
+	-Odilon Vieira</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="F13">
       <text>
         <t xml:space="preserve">Possibly 13, which was the number of nests analyzed by Stenzel &amp; Souza (2014), but the number of clutches was not specified.
@@ -1383,7 +1587,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>. (2003)</t>
+      <t>. (2013)</t>
     </r>
   </si>
   <si>

</xml_diff>

<commit_message>
add chart plot and other changes
</commit_message>
<xml_diff>
--- a/nesting_conopophagidae.xlsx
+++ b/nesting_conopophagidae.xlsx
@@ -17,6 +17,18 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="C53">
+      <text>
+        <t xml:space="preserve">Jorge Lizarazo in litt. (2023)
+	-Odilon Vieira</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="C52">
+      <text>
+        <t xml:space="preserve">Jorge Lizarazo in litt. (2023)
+	-Odilon Vieira</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="F27">
       <text>
         <t xml:space="preserve">"height of 40.6 ± 16.1 cm (range = 15–75) above the ground (N = 22).
@@ -3119,8 +3131,8 @@
       <c r="B52" s="5">
         <v>70.6</v>
       </c>
-      <c r="C52" s="15">
-        <v>4.95</v>
+      <c r="C52" s="5">
+        <v>49.5</v>
       </c>
       <c r="D52" s="15">
         <f>MEDIAN(107.4,121.5)</f>
@@ -3144,8 +3156,8 @@
         <f>MEDIAN(70.7,65.8)</f>
         <v>68.25</v>
       </c>
-      <c r="C53" s="15">
-        <v>3.9</v>
+      <c r="C53" s="5">
+        <v>39.1</v>
       </c>
       <c r="D53" s="15">
         <f>MEDIAN(132,112.3)</f>

</xml_diff>